<commit_message>
Changes on SPADE tests
</commit_message>
<xml_diff>
--- a/documentation/Test analysis.xlsx
+++ b/documentation/Test analysis.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\David\TFG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC82BC1-9FDF-4FCF-8BE0-B95A1EB2FF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FC3D37-19AC-4F78-9EC6-F34741A17CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A34D5EB-7974-4AB7-AA1E-C2DAAD35FC4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1A34D5EB-7974-4AB7-AA1E-C2DAAD35FC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
-    <sheet name="Test2" sheetId="2" r:id="rId2"/>
-    <sheet name="Test3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test2" sheetId="4" r:id="rId2"/>
+    <sheet name="Test3" sheetId="2" r:id="rId3"/>
+    <sheet name="Test4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="20">
   <si>
     <t>AGRESIVO</t>
   </si>
@@ -94,6 +95,9 @@
   </si>
   <si>
     <t>PRECIO MAXIMO DE PUJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -291,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -317,12 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,15 +328,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +345,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,8 +371,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA3BAD9"/>
       <color rgb="FF485B73"/>
-      <color rgb="FFA3BAD9"/>
       <color rgb="FFD5E5F2"/>
     </mruColors>
   </colors>
@@ -403,7 +410,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="485B73"/>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -438,7 +445,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="485B73"/>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -459,7 +466,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test2!$F$30</c:f>
+              <c:f>Test2!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -482,7 +489,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-86C8-412F-9A4D-A88B48231835}"/>
+                <c16:uniqueId val="{00000002-AFF7-4BC9-82A9-620D54B200F4}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -500,7 +507,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-86C8-412F-9A4D-A88B48231835}"/>
+                <c16:uniqueId val="{00000001-AFF7-4BC9-82A9-620D54B200F4}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -523,7 +530,7 @@
                     <a:solidFill>
                       <a:srgbClr val="D5E5F2"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -558,36 +565,36 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Test2!$G$29:$H$29</c:f>
+              <c:f>Test2!$C$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>TIMIDO</c:v>
+                  <c:v>RESTO</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AGRESIVO</c:v>
+                  <c:v>INFORMADO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Test2!$G$30:$H$30</c:f>
+              <c:f>Test2!$C$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-86C8-412F-9A4D-A88B48231835}"/>
+              <c16:uniqueId val="{00000000-AFF7-4BC9-82A9-620D54B200F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -706,6 +713,309 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
+                  <a:srgbClr val="485B73"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:srgbClr val="485B73"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Ganador</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="485B73"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Test3!$F$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GANADOR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="A3BAD9"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-86C8-412F-9A4D-A88B48231835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="485B73"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-86C8-412F-9A4D-A88B48231835}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="D5E5F2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Test3!$G$29:$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TIMIDO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AGRESIVO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Test3!$G$30:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-86C8-412F-9A4D-A88B48231835}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -781,7 +1091,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test2!$B$30</c:f>
+              <c:f>Test3!$B$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -875,7 +1185,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Test2!$C$29:$D$29</c:f>
+              <c:f>Test3!$C$29:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -889,7 +1199,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Test2!$C$30:$D$30</c:f>
+              <c:f>Test3!$C$30:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1031,7 +1341,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1110,7 +1420,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test3!$B$27</c:f>
+              <c:f>Test4!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1277,7 +1587,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Test3!$C$26:$D$26</c:f>
+              <c:f>Test4!$C$26:$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1291,7 +1601,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Test3!$C$27:$D$27</c:f>
+              <c:f>Test4!$C$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1521,6 +1831,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="255">
   <cs:axisTitle>
@@ -1990,7 +2340,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="220">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="255">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2458,7 +2808,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="255">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="220">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2925,7 +3275,516 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="255">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CCCDEF-E533-FF54-956B-C65F571AE6F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3006,7 +3865,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3346,8 +4205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5DE1F5-63EC-4627-B248-BF39D2211836}">
   <dimension ref="B2:T237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:O24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3358,20 +4217,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="2:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -3400,10 +4259,10 @@
       <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4179,10 +5038,10 @@
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O24" s="10" t="s">
+      <c r="O24" s="9" t="s">
         <v>0</v>
       </c>
       <c r="P24" s="2"/>
@@ -5958,11 +6817,265 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D630BCC8-2E6B-43A8-BC50-BBC282795EDC}">
+  <dimension ref="A2:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211C9B20-7DC3-4C1B-A42D-EE0978FFE7DB}">
   <dimension ref="B4:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5971,15 +7084,15 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="17"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
@@ -6356,27 +7469,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D9AA17-9985-4CE7-9154-9CCDC3B9BFD2}">
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4"/>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -6386,13 +7499,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6405,7 +7518,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>29</v>
       </c>
       <c r="G4" s="7">
@@ -6425,7 +7538,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>23.43</v>
       </c>
       <c r="G5" s="7">
@@ -6445,7 +7558,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>26</v>
       </c>
       <c r="G6" s="7">
@@ -6465,7 +7578,7 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>30</v>
       </c>
       <c r="G7" s="7">
@@ -6485,7 +7598,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>26</v>
       </c>
       <c r="G8" s="7">
@@ -6505,7 +7618,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>29</v>
       </c>
       <c r="G9" s="7">
@@ -6525,7 +7638,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>23.49</v>
       </c>
       <c r="G10" s="7">
@@ -6545,7 +7658,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>24</v>
       </c>
       <c r="G11" s="7">
@@ -6565,7 +7678,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>22</v>
       </c>
       <c r="G12" s="7">
@@ -6585,7 +7698,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>28</v>
       </c>
       <c r="G13" s="7">
@@ -6605,7 +7718,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>26</v>
       </c>
       <c r="G14" s="7">
@@ -6625,7 +7738,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <v>27</v>
       </c>
       <c r="G15" s="7">
@@ -6645,7 +7758,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>29</v>
       </c>
       <c r="G16" s="7">
@@ -6665,7 +7778,7 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <v>25</v>
       </c>
       <c r="G17" s="7">
@@ -6685,7 +7798,7 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="12">
+      <c r="F18" s="10">
         <v>30</v>
       </c>
       <c r="G18" s="7">
@@ -6705,7 +7818,7 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="12">
+      <c r="F19" s="10">
         <v>27.79</v>
       </c>
       <c r="G19" s="7">
@@ -6725,7 +7838,7 @@
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <v>26.08</v>
       </c>
       <c r="G20" s="7">
@@ -6745,7 +7858,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="12">
+      <c r="F21" s="10">
         <v>27</v>
       </c>
       <c r="G21" s="7">
@@ -6765,7 +7878,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <v>30</v>
       </c>
       <c r="G22" s="7">
@@ -6785,7 +7898,7 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="12">
+      <c r="F23" s="10">
         <v>26</v>
       </c>
       <c r="G23" s="7">
@@ -6805,13 +7918,13 @@
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <v>29</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <v>29</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6821,11 +7934,11 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="10">
+      <c r="G25" s="22"/>
+      <c r="H25" s="9">
         <f>AVERAGE(H4:H24)</f>
         <v>1.3433333333333335</v>
       </c>

</xml_diff>